<commit_message>
alterei css e js de pasta e fiz alterações para passar todos os nomes da lista para o banco
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -477,6 +477,424 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>terqui1415</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2024-06-15</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>paulo</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>r, a, f, a, e, l</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>segqua2122</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2024-06-16</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>pedro</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>t, h, a, l, e, s</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>segqua2122</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2024-06-16</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>pedro</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>t, h, a, l, e, s</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>terqui0910</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2024-06-18</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>julio</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>n, a, t, a, s, h, a</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>segqua0708</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2024-06-18</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>paulo</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>p, i, p, i, c, o</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>terqui1415</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>2024-06-30</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>julio</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>rafael</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>terqui1415</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>2024-06-30</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>julio</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>rafael</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>terqui1415</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>2024-06-30</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>julio</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>rafael</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>terqui1415</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>2024-06-30</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>julio</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>rafael</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>terqui1415</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>2024-06-30</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>julio</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>rafael</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>terqui1415</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>2024-06-26</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>julio</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>jennifer</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>terqui1314</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>2024-06-26</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>julio</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>jennifer</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>terqui1415</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>2024-06-24</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>pedro</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>jennifer, luiz</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>terqui1415</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>2024-06-24</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>pedro</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>jennifer, luiz</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>segqua2122</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>2024-06-26</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>julio</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>thales, letícia</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>segqua1112</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>2024-06-14</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>julio</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>andré</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>segqua0708</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>2024-06-30</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>pedro</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>manel, bernardo, pipico</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>segqua0708</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>2024-06-16</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>pedro</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Manel, Bernardo, Pipico</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>segqua2122</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>2024-06-11</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>pedro</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Thales, Amanda</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
including env variables and git ignore
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -917,6 +917,28 @@
         </is>
       </c>
     </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>segqua0708</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>2024-06-12</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>julio</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Manel, Bernardo</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>